<commit_message>
comment and legal documents in progress
</commit_message>
<xml_diff>
--- a/doc/preseed/preseed-budget.xlsx
+++ b/doc/preseed/preseed-budget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="0" windowWidth="32880" windowHeight="24000" tabRatio="163"/>
+    <workbookView xWindow="24540" yWindow="8180" windowWidth="25360" windowHeight="15820" tabRatio="163"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
-    <t>aug</t>
-  </si>
-  <si>
     <t>Oct</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>accumulated</t>
+  </si>
+  <si>
+    <t>Sep</t>
   </si>
 </sst>
 </file>
@@ -87,7 +87,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -96,6 +96,20 @@
     <font>
       <b/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -117,8 +131,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -126,7 +142,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Besøgt link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -509,7 +527,7 @@
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -519,27 +537,27 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -560,7 +578,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2">
         <v>4000</v>
@@ -584,7 +602,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2">
         <v>1000</v>
@@ -608,7 +626,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2">
         <v>1000</v>
@@ -650,7 +668,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -671,7 +689,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="2">
         <v>7000</v>
@@ -695,7 +713,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="2">
         <v>1000</v>
@@ -719,7 +737,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="2">
         <v>0</v>
@@ -761,7 +779,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -782,7 +800,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" s="2">
         <v>1500</v>
@@ -842,7 +860,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -863,7 +881,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" s="2">
         <v>1500</v>
@@ -914,7 +932,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C31" s="2">
         <v>1000</v>
@@ -947,12 +965,12 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C35" s="2">
         <v>1000</v>
@@ -975,7 +993,7 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C38" s="2">
         <f t="shared" ref="C38:H38" si="0">C6+C7+C8+C13+C14+C15+C20+C27+C31+C35</f>
@@ -1004,7 +1022,7 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C40" s="2">
         <f>C38</f>

</xml_diff>